<commit_message>
B class instances added
</commit_message>
<xml_diff>
--- a/Resultados TCP Final.xlsx
+++ b/Resultados TCP Final.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050"/>
   </bookViews>
   <sheets>
-    <sheet name="D" sheetId="4" r:id="rId1"/>
-    <sheet name="C" sheetId="3" r:id="rId2"/>
-    <sheet name="B" sheetId="2" r:id="rId3"/>
-    <sheet name="A" sheetId="1" r:id="rId4"/>
-    <sheet name="S" sheetId="7" r:id="rId5"/>
-    <sheet name="SS" sheetId="8" r:id="rId6"/>
-    <sheet name="SSS" sheetId="9" r:id="rId7"/>
+    <sheet name="E" sheetId="10" r:id="rId1"/>
+    <sheet name="D" sheetId="4" r:id="rId2"/>
+    <sheet name="C" sheetId="3" r:id="rId3"/>
+    <sheet name="B" sheetId="2" r:id="rId4"/>
+    <sheet name="A" sheetId="1" r:id="rId5"/>
+    <sheet name="S" sheetId="7" r:id="rId6"/>
+    <sheet name="SS" sheetId="8" r:id="rId7"/>
+    <sheet name="SSS" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="93">
   <si>
     <t>instance</t>
   </si>
@@ -236,6 +237,69 @@
   </si>
   <si>
     <t>steine09</t>
+  </si>
+  <si>
+    <t>\\steinb01</t>
+  </si>
+  <si>
+    <t>\\steinb02</t>
+  </si>
+  <si>
+    <t>\\steinb03</t>
+  </si>
+  <si>
+    <t>\\steinb04</t>
+  </si>
+  <si>
+    <t>\\steinb05</t>
+  </si>
+  <si>
+    <t>\\steinb06</t>
+  </si>
+  <si>
+    <t>\\steinb07</t>
+  </si>
+  <si>
+    <t>\\steinb08</t>
+  </si>
+  <si>
+    <t>\\steinb09</t>
+  </si>
+  <si>
+    <t>\\steinb10</t>
+  </si>
+  <si>
+    <t>\\steinb11</t>
+  </si>
+  <si>
+    <t>\\steinb12</t>
+  </si>
+  <si>
+    <t>\\steinb13</t>
+  </si>
+  <si>
+    <t>\\steinb14</t>
+  </si>
+  <si>
+    <t>\\steinb15</t>
+  </si>
+  <si>
+    <t>\\steinb16</t>
+  </si>
+  <si>
+    <t>\\steinb17</t>
+  </si>
+  <si>
+    <t>\\steinb18</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -575,6 +639,756 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>83</v>
+      </c>
+      <c r="C2">
+        <v>83</v>
+      </c>
+      <c r="D2">
+        <v>83</v>
+      </c>
+      <c r="E2">
+        <v>83</v>
+      </c>
+      <c r="F2">
+        <v>163.80000000000001</v>
+      </c>
+      <c r="G2">
+        <v>91.7</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3">
+        <v>83</v>
+      </c>
+      <c r="C3">
+        <v>83</v>
+      </c>
+      <c r="D3">
+        <v>83</v>
+      </c>
+      <c r="E3">
+        <v>83</v>
+      </c>
+      <c r="F3">
+        <v>124.5</v>
+      </c>
+      <c r="G3">
+        <v>14.6</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4">
+        <v>138</v>
+      </c>
+      <c r="C4">
+        <v>138</v>
+      </c>
+      <c r="D4">
+        <v>138</v>
+      </c>
+      <c r="E4">
+        <v>138</v>
+      </c>
+      <c r="F4">
+        <v>218.7</v>
+      </c>
+      <c r="G4" s="1">
+        <v>95.9</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5">
+        <v>59</v>
+      </c>
+      <c r="C5">
+        <v>59</v>
+      </c>
+      <c r="D5">
+        <v>59</v>
+      </c>
+      <c r="E5">
+        <v>59</v>
+      </c>
+      <c r="F5">
+        <v>129.30000000000001</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6">
+        <v>61</v>
+      </c>
+      <c r="C6">
+        <v>61</v>
+      </c>
+      <c r="D6">
+        <v>61</v>
+      </c>
+      <c r="E6">
+        <v>61</v>
+      </c>
+      <c r="F6">
+        <v>253.5</v>
+      </c>
+      <c r="G6">
+        <v>128.19999999999999</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7">
+        <v>125</v>
+      </c>
+      <c r="C7">
+        <v>125</v>
+      </c>
+      <c r="D7">
+        <v>125</v>
+      </c>
+      <c r="E7">
+        <v>125</v>
+      </c>
+      <c r="F7">
+        <v>330.5</v>
+      </c>
+      <c r="G7">
+        <v>191.1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8">
+        <v>111</v>
+      </c>
+      <c r="C8">
+        <v>112</v>
+      </c>
+      <c r="D8">
+        <v>111.1</v>
+      </c>
+      <c r="E8">
+        <v>111</v>
+      </c>
+      <c r="F8">
+        <v>237.5</v>
+      </c>
+      <c r="G8">
+        <v>100.6</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9">
+        <v>107</v>
+      </c>
+      <c r="C9">
+        <v>107</v>
+      </c>
+      <c r="D9">
+        <v>107</v>
+      </c>
+      <c r="E9">
+        <v>107</v>
+      </c>
+      <c r="F9">
+        <v>140.9</v>
+      </c>
+      <c r="G9" s="1">
+        <v>14.1</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>221</v>
+      </c>
+      <c r="C10">
+        <v>221</v>
+      </c>
+      <c r="D10">
+        <v>221</v>
+      </c>
+      <c r="E10">
+        <v>221</v>
+      </c>
+      <c r="F10">
+        <v>165.6</v>
+      </c>
+      <c r="G10">
+        <v>0.5</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11">
+        <v>88</v>
+      </c>
+      <c r="C11">
+        <v>88</v>
+      </c>
+      <c r="D11">
+        <v>88</v>
+      </c>
+      <c r="E11">
+        <v>88</v>
+      </c>
+      <c r="F11">
+        <v>342.2</v>
+      </c>
+      <c r="G11">
+        <v>159.6</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>7</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12">
+        <v>88</v>
+      </c>
+      <c r="C12">
+        <v>88</v>
+      </c>
+      <c r="D12">
+        <v>88</v>
+      </c>
+      <c r="E12">
+        <v>88</v>
+      </c>
+      <c r="F12">
+        <v>380.7</v>
+      </c>
+      <c r="G12">
+        <v>194.9</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13">
+        <v>174</v>
+      </c>
+      <c r="C13">
+        <v>176</v>
+      </c>
+      <c r="D13">
+        <v>174.9</v>
+      </c>
+      <c r="E13">
+        <v>175</v>
+      </c>
+      <c r="F13">
+        <v>513</v>
+      </c>
+      <c r="G13">
+        <v>327.10000000000002</v>
+      </c>
+      <c r="H13">
+        <v>9</v>
+      </c>
+      <c r="I13">
+        <v>11</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14">
+        <v>173</v>
+      </c>
+      <c r="C14">
+        <v>174</v>
+      </c>
+      <c r="D14">
+        <v>173.9</v>
+      </c>
+      <c r="E14">
+        <v>174</v>
+      </c>
+      <c r="F14">
+        <v>261.5</v>
+      </c>
+      <c r="G14">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="H14">
+        <v>14</v>
+      </c>
+      <c r="I14">
+        <v>17</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15">
+        <v>239</v>
+      </c>
+      <c r="C15">
+        <v>239</v>
+      </c>
+      <c r="D15">
+        <v>239</v>
+      </c>
+      <c r="E15">
+        <v>239</v>
+      </c>
+      <c r="F15">
+        <v>490.7</v>
+      </c>
+      <c r="G15">
+        <v>261.8</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <v>11</v>
+      </c>
+      <c r="K15">
+        <v>11</v>
+      </c>
+      <c r="L15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16">
+        <v>325</v>
+      </c>
+      <c r="C16">
+        <v>328</v>
+      </c>
+      <c r="D16">
+        <v>325.75</v>
+      </c>
+      <c r="E16">
+        <v>325</v>
+      </c>
+      <c r="F16">
+        <v>688.5</v>
+      </c>
+      <c r="G16">
+        <v>417.75</v>
+      </c>
+      <c r="H16">
+        <v>12</v>
+      </c>
+      <c r="I16">
+        <v>14</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17">
+        <v>127</v>
+      </c>
+      <c r="C17">
+        <v>130</v>
+      </c>
+      <c r="D17">
+        <v>128.5</v>
+      </c>
+      <c r="E17">
+        <v>128.5</v>
+      </c>
+      <c r="F17">
+        <v>518.1</v>
+      </c>
+      <c r="G17">
+        <v>279.2</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>16</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18">
+        <v>132</v>
+      </c>
+      <c r="C18">
+        <v>142</v>
+      </c>
+      <c r="D18">
+        <v>133.4</v>
+      </c>
+      <c r="E18">
+        <v>132</v>
+      </c>
+      <c r="F18">
+        <v>545.4</v>
+      </c>
+      <c r="G18">
+        <v>418.4</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <v>11</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+      <c r="K18">
+        <v>8</v>
+      </c>
+      <c r="L18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19">
+        <v>218</v>
+      </c>
+      <c r="C19">
+        <v>219</v>
+      </c>
+      <c r="D19">
+        <v>218.9</v>
+      </c>
+      <c r="E19">
+        <v>219</v>
+      </c>
+      <c r="F19">
+        <v>514</v>
+      </c>
+      <c r="G19">
+        <v>268.89999999999998</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>8</v>
+      </c>
+      <c r="L19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f>AVERAGE(F2:F19)</f>
+        <v>334.35555555555555</v>
+      </c>
+      <c r="G20">
+        <f>AVERAGE(G2:G19)</f>
+        <v>168.65277777777777</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L62"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
@@ -2916,7 +3730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L62"/>
   <sheetViews>
@@ -5263,7 +6077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L62"/>
   <sheetViews>
@@ -7610,7 +8424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L62"/>
   <sheetViews>
@@ -9960,7 +10774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L62"/>
   <sheetViews>
@@ -12310,7 +13124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L62"/>
   <sheetViews>
@@ -14649,11 +15463,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>

</xml_diff>